<commit_message>
perbaruan laporan sampe bab 2
</commit_message>
<xml_diff>
--- a/DATA SET/ResponGoogleForm.xlsx
+++ b/DATA SET/ResponGoogleForm.xlsx
@@ -1,22 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Kuliah\Semester 6\TUGAS AKHIR\DATA SET\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB06499-BB06-422B-9F80-90604BA2CE30}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="630" windowWidth="19635" windowHeight="7440"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="299">
   <si>
     <t>Beberapa dosen kadang kurang menguasai materi yang akan diberikan. Cara ajar dosen yang kurang kreatif</t>
   </si>
@@ -31,10 +44,6 @@
   </si>
   <si>
     <t>Dosen harap fast respon</t>
-  </si>
-  <si>
-    <t>Kenapa jadwal TI lebih padat dibandingkan Jurusan lain? Padahal jumlah SKS nya sama. 
-Dan untuk dosen, ada beberapa dosen yang mengajar itu seenaknya saja. Tidak memperhatikan kemampuan masing2 mahasiswanya. Menjelaskan materi yang jadi patokan hanya pada mahasiswa yang mengerti saja. Saat tubes tidak mau melihat prosesnya tapi hanya melihat hasil akhirnya saja, belum tentu tubesnya buatan sendiri. Memberi nilai tergantung pada suatu alasan.</t>
   </si>
   <si>
     <t>Jangan anggap kami mahasiswa, paham semua ketika dijelasin oleh bapak atau ibu dosen</t>
@@ -68,9 +77,6 @@
     <t>Jam belajar kurang</t>
   </si>
   <si>
-    <t>infomasi yang slalu serba tiba" dalam hal apapun. untuk dosen kurangnya motivasi terhadap mahasiswa dan menyakinkan mahasiswa tapi bukan berarti terlalu menekan juga</t>
-  </si>
-  <si>
     <t>Dosen yang masih menggunakan metode belajar kurikulum 2013. Membuat pembelajaran tidak lengkap dan jelas.</t>
   </si>
   <si>
@@ -333,9 +339,6 @@
     <t>KELUHAN</t>
   </si>
   <si>
-    <t>LABEL</t>
-  </si>
-  <si>
     <t>Negatif</t>
   </si>
   <si>
@@ -343,9 +346,6 @@
   </si>
   <si>
     <t>Sudah bagus kok</t>
-  </si>
-  <si>
-    <t>Pelayanannya baik</t>
   </si>
   <si>
     <t>Saya rasa bagian keuangan sudah cukup baik</t>
@@ -899,12 +899,42 @@
   </si>
   <si>
     <t>Unit kegiatan mahasiswa sangat membantu kemampuan mahasiswa untuk berorganisasi</t>
+  </si>
+  <si>
+    <t>KATEGORI</t>
+  </si>
+  <si>
+    <t>TENAGA PENGAJAR (DOSEN)</t>
+  </si>
+  <si>
+    <t>SENTIMEN</t>
+  </si>
+  <si>
+    <t>AKADEMIK</t>
+  </si>
+  <si>
+    <t>Beberapa dosen yang mengajar itu seenaknya saja. Tidak memperhatikan kemampuan masing2 mahasiswanya. Menjelaskan materi yang jadi patokan hanya pada mahasiswa yang mengerti saja. Saat tubes tidak mau melihat prosesnya tapi hanya melihat hasil akhirnya saja, belum tentu tubesnya buatan sendiri. Memberi nilai tergantung pada suatu alasan.</t>
+  </si>
+  <si>
+    <t>SARANA PRASARANA</t>
+  </si>
+  <si>
+    <t>Untuk dosen kurangnya motivasi terhadap mahasiswa dan menyakinkan mahasiswa tapi bukan berarti terlalu menekan juga</t>
+  </si>
+  <si>
+    <t>KEUANGAN</t>
+  </si>
+  <si>
+    <t>LAINNYA</t>
+  </si>
+  <si>
+    <t>Pelayanan bagian keuangan sudah baik, karena selalu ada ketika dibutuhkan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -951,6 +981,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -999,7 +1032,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1032,9 +1065,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1067,6 +1117,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1242,30 +1309,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C301"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B275" workbookViewId="0">
-      <selection activeCell="B288" sqref="B288"/>
+    <sheetView tabSelected="1" topLeftCell="C24" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1273,10 +1344,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="D2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>(A2+1)</f>
         <v>2</v>
@@ -1285,10 +1359,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="D3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f t="shared" ref="A4:A67" si="0">(A3+1)</f>
         <v>3</v>
@@ -1297,10 +1374,13 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="D4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1309,22 +1389,28 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="D5" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="D6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1333,499 +1419,601 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="D7" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <f t="shared" si="0"/>
+      <c r="C9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <f t="shared" si="0"/>
+      <c r="C12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <f t="shared" si="0"/>
+      <c r="C13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <f t="shared" si="0"/>
+      <c r="C15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <f t="shared" si="0"/>
+      <c r="C16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <f t="shared" si="0"/>
+      <c r="C17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C14" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <f t="shared" si="0"/>
+      <c r="C18" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <f t="shared" si="0"/>
+      <c r="C19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <f t="shared" si="0"/>
+      <c r="C21" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <f t="shared" si="0"/>
+      <c r="C22" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <f t="shared" si="0"/>
+      <c r="C23" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <f t="shared" si="0"/>
+      <c r="C24" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <f t="shared" si="0"/>
+      <c r="C25" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <f t="shared" si="0"/>
+      <c r="C26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <f t="shared" si="0"/>
+      <c r="C27" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <f t="shared" si="0"/>
+      <c r="C28" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <f t="shared" si="0"/>
+      <c r="C29" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <f t="shared" si="0"/>
+      <c r="C30" t="s">
+        <v>102</v>
+      </c>
+      <c r="D30" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <f t="shared" si="0"/>
+      <c r="C31" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <f t="shared" si="0"/>
+      <c r="C32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D32" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <f t="shared" si="0"/>
+      <c r="C33" t="s">
+        <v>102</v>
+      </c>
+      <c r="D33" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" t="s">
+        <v>103</v>
+      </c>
+      <c r="D34" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <f t="shared" si="0"/>
+      <c r="C35" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <f t="shared" si="0"/>
+      <c r="C36" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <f t="shared" si="0"/>
+      <c r="C37" t="s">
+        <v>102</v>
+      </c>
+      <c r="D37" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <f t="shared" si="0"/>
+      <c r="C38" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>298</v>
+      </c>
+      <c r="C39" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <f t="shared" si="0"/>
+      <c r="C40" t="s">
+        <v>102</v>
+      </c>
+      <c r="D40" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C34" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
-        <f t="shared" si="0"/>
+      <c r="C41" t="s">
+        <v>102</v>
+      </c>
+      <c r="D41" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
-        <f t="shared" si="0"/>
+      <c r="C42" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C36" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
-        <f t="shared" si="0"/>
+      <c r="C43" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
-        <f t="shared" si="0"/>
+      <c r="C44" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>116</v>
+      </c>
+      <c r="C45" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C38" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
-        <f t="shared" si="0"/>
+      <c r="C46" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
         <v>38</v>
       </c>
-      <c r="B39" t="s">
-        <v>108</v>
-      </c>
-      <c r="C39" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
-        <f t="shared" si="0"/>
+      <c r="C47" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C40" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="B41" t="s">
-        <v>35</v>
-      </c>
-      <c r="C41" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="B43" t="s">
-        <v>37</v>
-      </c>
-      <c r="C43" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C44" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="B45" t="s">
-        <v>120</v>
-      </c>
-      <c r="C45" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C46" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="B47" t="s">
-        <v>40</v>
-      </c>
-      <c r="C47" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="B48" t="s">
-        <v>41</v>
-      </c>
       <c r="C48" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1834,10 +2022,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C49" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1846,10 +2034,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C50" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1858,10 +2046,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C51" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1870,10 +2058,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C52" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1882,10 +2070,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C53" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1894,10 +2082,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C54" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1906,10 +2094,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C55" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1918,10 +2106,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C56" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1930,10 +2118,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C57" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1942,10 +2130,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C58" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1954,10 +2142,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C59" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1966,10 +2154,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C60" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1978,10 +2166,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C61" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1990,10 +2178,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C62" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -2002,10 +2190,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C63" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -2014,10 +2202,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C64" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -2026,10 +2214,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C65" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -2038,10 +2226,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C66" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -2050,10 +2238,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C67" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -2062,10 +2250,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C68" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -2074,10 +2262,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C69" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -2086,10 +2274,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C70" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -2098,10 +2286,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C71" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -2110,10 +2298,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C72" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -2122,10 +2310,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C73" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -2134,10 +2322,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C74" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -2146,10 +2334,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C75" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -2158,10 +2346,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C76" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -2170,10 +2358,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C77" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -2182,10 +2370,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C78" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -2194,10 +2382,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C79" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -2206,10 +2394,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C80" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -2218,10 +2406,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C81" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -2230,10 +2418,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C82" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -2242,10 +2430,10 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C83" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -2254,10 +2442,10 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C84" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -2266,10 +2454,10 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C85" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -2278,10 +2466,10 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C86" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -2290,10 +2478,10 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C87" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -2302,10 +2490,10 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C88" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -2314,10 +2502,10 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C89" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -2326,10 +2514,10 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C90" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -2338,10 +2526,10 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C91" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -2350,10 +2538,10 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C92" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -2362,10 +2550,10 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C93" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -2374,10 +2562,10 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C94" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -2386,10 +2574,10 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C95" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -2398,10 +2586,10 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C96" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -2410,10 +2598,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C97" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -2422,10 +2610,10 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C98" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -2434,10 +2622,10 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C99" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -2446,10 +2634,10 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C100" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -2458,10 +2646,10 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C101" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -2470,10 +2658,10 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C102" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -2482,10 +2670,10 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C103" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -2494,10 +2682,10 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C104" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -2506,10 +2694,10 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C105" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -2518,10 +2706,10 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C106" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -2530,10 +2718,10 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C107" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -2542,10 +2730,10 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C108" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -2554,10 +2742,10 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C109" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -2566,10 +2754,10 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C110" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -2578,10 +2766,10 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C111" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -2590,10 +2778,10 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C112" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -2602,10 +2790,10 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C113" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -2614,10 +2802,10 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C114" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -2626,10 +2814,10 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C115" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -2638,10 +2826,10 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C116" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -2650,10 +2838,10 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C117" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -2662,10 +2850,10 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C118" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -2674,10 +2862,10 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C119" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -2686,10 +2874,10 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C120" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -2698,10 +2886,10 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C121" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -2710,10 +2898,10 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C122" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -2722,10 +2910,10 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C123" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -2734,10 +2922,10 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C124" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -2746,10 +2934,10 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C125" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -2758,10 +2946,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C126" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -2770,10 +2958,10 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C127" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -2782,10 +2970,10 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C128" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -2794,10 +2982,10 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C129" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -2806,10 +2994,10 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C130" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -2818,10 +3006,10 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C131" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -2830,10 +3018,10 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C132" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -2842,10 +3030,10 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C133" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -2854,10 +3042,10 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C134" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -2866,10 +3054,10 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C135" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -2878,10 +3066,10 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C136" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -2890,10 +3078,10 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C137" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -2902,10 +3090,10 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C138" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -2914,10 +3102,10 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C139" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -2926,10 +3114,10 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C140" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -2938,10 +3126,10 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C141" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -2950,10 +3138,10 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C142" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -2962,10 +3150,10 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C143" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -2974,10 +3162,10 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C144" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -2986,10 +3174,10 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C145" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -2998,10 +3186,10 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C146" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -3010,10 +3198,10 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C147" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -3022,10 +3210,10 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C148" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -3034,10 +3222,10 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C149" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -3046,10 +3234,10 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C150" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -3058,10 +3246,10 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C151" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -3070,10 +3258,10 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C152" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -3082,10 +3270,10 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C153" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -3094,10 +3282,10 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C154" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -3106,10 +3294,10 @@
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C155" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -3118,10 +3306,10 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C156" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -3130,10 +3318,10 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C157" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -3142,10 +3330,10 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C158" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -3154,10 +3342,10 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C159" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -3166,10 +3354,10 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C160" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -3178,10 +3366,10 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C161" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -3190,10 +3378,10 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C162" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -3202,10 +3390,10 @@
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C163" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -3214,10 +3402,10 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C164" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -3226,10 +3414,10 @@
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C165" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -3238,10 +3426,10 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C166" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -3250,10 +3438,10 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C167" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -3262,10 +3450,10 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C168" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -3274,10 +3462,10 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C169" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -3286,10 +3474,10 @@
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C170" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -3298,10 +3486,10 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C171" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -3310,10 +3498,10 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C172" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -3322,10 +3510,10 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C173" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -3334,10 +3522,10 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C174" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -3346,10 +3534,10 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C175" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -3358,10 +3546,10 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C176" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -3370,10 +3558,10 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C177" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -3382,10 +3570,10 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C178" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -3394,10 +3582,10 @@
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C179" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -3406,10 +3594,10 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C180" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -3418,10 +3606,10 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C181" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -3430,10 +3618,10 @@
         <v>181</v>
       </c>
       <c r="B182" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C182" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -3442,10 +3630,10 @@
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C183" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -3454,10 +3642,10 @@
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C184" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -3466,10 +3654,10 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C185" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
@@ -3478,10 +3666,10 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C186" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
@@ -3490,10 +3678,10 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C187" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -3502,10 +3690,10 @@
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C188" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
@@ -3514,10 +3702,10 @@
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C189" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -3526,10 +3714,10 @@
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C190" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
@@ -3538,10 +3726,10 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C191" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
@@ -3550,10 +3738,10 @@
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C192" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
@@ -3562,10 +3750,10 @@
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C193" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -3574,10 +3762,10 @@
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C194" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -3586,10 +3774,10 @@
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C195" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -3598,10 +3786,10 @@
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C196" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -3610,10 +3798,10 @@
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C197" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -3622,10 +3810,10 @@
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C198" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -3634,10 +3822,10 @@
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C199" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -3646,10 +3834,10 @@
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C200" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -3658,10 +3846,10 @@
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C201" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
@@ -3670,10 +3858,10 @@
         <v>201</v>
       </c>
       <c r="B202" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C202" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
@@ -3682,10 +3870,10 @@
         <v>202</v>
       </c>
       <c r="B203" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C203" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -3694,10 +3882,10 @@
         <v>203</v>
       </c>
       <c r="B204" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C204" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -3706,10 +3894,10 @@
         <v>204</v>
       </c>
       <c r="B205" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C205" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
@@ -3718,10 +3906,10 @@
         <v>205</v>
       </c>
       <c r="B206" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C206" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
@@ -3730,10 +3918,10 @@
         <v>206</v>
       </c>
       <c r="B207" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C207" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
@@ -3742,10 +3930,10 @@
         <v>207</v>
       </c>
       <c r="B208" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C208" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
@@ -3754,10 +3942,10 @@
         <v>208</v>
       </c>
       <c r="B209" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C209" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -3766,10 +3954,10 @@
         <v>209</v>
       </c>
       <c r="B210" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C210" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -3778,10 +3966,10 @@
         <v>210</v>
       </c>
       <c r="B211" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C211" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
@@ -3790,10 +3978,10 @@
         <v>211</v>
       </c>
       <c r="B212" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C212" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
@@ -3802,10 +3990,10 @@
         <v>212</v>
       </c>
       <c r="B213" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C213" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
@@ -3814,10 +4002,10 @@
         <v>213</v>
       </c>
       <c r="B214" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C214" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
@@ -3826,10 +4014,10 @@
         <v>214</v>
       </c>
       <c r="B215" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C215" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
@@ -3838,10 +4026,10 @@
         <v>215</v>
       </c>
       <c r="B216" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C216" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
@@ -3850,10 +4038,10 @@
         <v>216</v>
       </c>
       <c r="B217" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C217" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
@@ -3862,10 +4050,10 @@
         <v>217</v>
       </c>
       <c r="B218" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C218" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
@@ -3874,10 +4062,10 @@
         <v>218</v>
       </c>
       <c r="B219" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C219" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
@@ -3886,10 +4074,10 @@
         <v>219</v>
       </c>
       <c r="B220" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C220" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
@@ -3898,10 +4086,10 @@
         <v>220</v>
       </c>
       <c r="B221" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C221" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
@@ -3910,10 +4098,10 @@
         <v>221</v>
       </c>
       <c r="B222" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C222" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
@@ -3922,10 +4110,10 @@
         <v>222</v>
       </c>
       <c r="B223" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C223" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
@@ -3934,10 +4122,10 @@
         <v>223</v>
       </c>
       <c r="B224" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C224" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -3946,10 +4134,10 @@
         <v>224</v>
       </c>
       <c r="B225" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C225" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
@@ -3958,10 +4146,10 @@
         <v>225</v>
       </c>
       <c r="B226" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C226" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
@@ -3970,10 +4158,10 @@
         <v>226</v>
       </c>
       <c r="B227" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C227" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
@@ -3982,10 +4170,10 @@
         <v>227</v>
       </c>
       <c r="B228" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C228" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
@@ -3994,10 +4182,10 @@
         <v>228</v>
       </c>
       <c r="B229" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C229" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
@@ -4006,10 +4194,10 @@
         <v>229</v>
       </c>
       <c r="B230" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C230" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
@@ -4018,10 +4206,10 @@
         <v>230</v>
       </c>
       <c r="B231" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C231" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
@@ -4030,10 +4218,10 @@
         <v>231</v>
       </c>
       <c r="B232" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C232" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
@@ -4042,10 +4230,10 @@
         <v>232</v>
       </c>
       <c r="B233" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C233" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
@@ -4054,10 +4242,10 @@
         <v>233</v>
       </c>
       <c r="B234" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C234" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
@@ -4066,10 +4254,10 @@
         <v>234</v>
       </c>
       <c r="B235" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C235" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
@@ -4078,10 +4266,10 @@
         <v>235</v>
       </c>
       <c r="B236" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C236" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
@@ -4090,10 +4278,10 @@
         <v>236</v>
       </c>
       <c r="B237" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C237" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
@@ -4102,10 +4290,10 @@
         <v>237</v>
       </c>
       <c r="B238" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C238" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
@@ -4114,10 +4302,10 @@
         <v>238</v>
       </c>
       <c r="B239" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C239" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
@@ -4126,10 +4314,10 @@
         <v>239</v>
       </c>
       <c r="B240" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C240" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
@@ -4138,10 +4326,10 @@
         <v>240</v>
       </c>
       <c r="B241" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C241" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
@@ -4150,10 +4338,10 @@
         <v>241</v>
       </c>
       <c r="B242" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C242" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
@@ -4162,10 +4350,10 @@
         <v>242</v>
       </c>
       <c r="B243" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C243" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
@@ -4174,10 +4362,10 @@
         <v>243</v>
       </c>
       <c r="B244" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C244" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
@@ -4186,10 +4374,10 @@
         <v>244</v>
       </c>
       <c r="B245" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C245" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
@@ -4198,10 +4386,10 @@
         <v>245</v>
       </c>
       <c r="B246" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C246" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
@@ -4210,10 +4398,10 @@
         <v>246</v>
       </c>
       <c r="B247" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C247" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
@@ -4222,10 +4410,10 @@
         <v>247</v>
       </c>
       <c r="B248" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C248" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
@@ -4234,10 +4422,10 @@
         <v>248</v>
       </c>
       <c r="B249" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C249" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
@@ -4246,10 +4434,10 @@
         <v>249</v>
       </c>
       <c r="B250" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C250" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
@@ -4258,10 +4446,10 @@
         <v>250</v>
       </c>
       <c r="B251" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C251" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
@@ -4270,10 +4458,10 @@
         <v>251</v>
       </c>
       <c r="B252" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C252" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
@@ -4282,10 +4470,10 @@
         <v>252</v>
       </c>
       <c r="B253" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C253" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
@@ -4294,10 +4482,10 @@
         <v>253</v>
       </c>
       <c r="B254" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C254" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
@@ -4306,10 +4494,10 @@
         <v>254</v>
       </c>
       <c r="B255" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C255" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
@@ -4318,10 +4506,10 @@
         <v>255</v>
       </c>
       <c r="B256" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C256" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
@@ -4330,10 +4518,10 @@
         <v>256</v>
       </c>
       <c r="B257" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C257" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
@@ -4342,10 +4530,10 @@
         <v>257</v>
       </c>
       <c r="B258" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C258" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
@@ -4354,10 +4542,10 @@
         <v>258</v>
       </c>
       <c r="B259" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C259" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
@@ -4366,10 +4554,10 @@
         <v>259</v>
       </c>
       <c r="B260" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C260" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
@@ -4378,10 +4566,10 @@
         <v>260</v>
       </c>
       <c r="B261" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C261" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
@@ -4390,10 +4578,10 @@
         <v>261</v>
       </c>
       <c r="B262" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C262" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
@@ -4402,10 +4590,10 @@
         <v>262</v>
       </c>
       <c r="B263" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C263" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
@@ -4414,10 +4602,10 @@
         <v>263</v>
       </c>
       <c r="B264" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C264" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
@@ -4426,10 +4614,10 @@
         <v>264</v>
       </c>
       <c r="B265" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C265" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
@@ -4438,10 +4626,10 @@
         <v>265</v>
       </c>
       <c r="B266" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C266" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
@@ -4450,10 +4638,10 @@
         <v>266</v>
       </c>
       <c r="B267" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C267" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
@@ -4462,10 +4650,10 @@
         <v>267</v>
       </c>
       <c r="B268" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C268" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
@@ -4474,10 +4662,10 @@
         <v>268</v>
       </c>
       <c r="B269" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C269" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
@@ -4486,10 +4674,10 @@
         <v>269</v>
       </c>
       <c r="B270" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C270" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
@@ -4498,10 +4686,10 @@
         <v>270</v>
       </c>
       <c r="B271" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C271" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
@@ -4510,10 +4698,10 @@
         <v>271</v>
       </c>
       <c r="B272" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C272" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
@@ -4522,10 +4710,10 @@
         <v>272</v>
       </c>
       <c r="B273" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C273" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
@@ -4534,10 +4722,10 @@
         <v>273</v>
       </c>
       <c r="B274" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C274" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
@@ -4546,10 +4734,10 @@
         <v>274</v>
       </c>
       <c r="B275" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C275" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
@@ -4558,10 +4746,10 @@
         <v>275</v>
       </c>
       <c r="B276" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C276" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
@@ -4570,10 +4758,10 @@
         <v>276</v>
       </c>
       <c r="B277" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C277" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
@@ -4582,10 +4770,10 @@
         <v>277</v>
       </c>
       <c r="B278" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C278" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
@@ -4594,10 +4782,10 @@
         <v>278</v>
       </c>
       <c r="B279" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C279" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
@@ -4606,10 +4794,10 @@
         <v>279</v>
       </c>
       <c r="B280" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C280" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
@@ -4618,10 +4806,10 @@
         <v>280</v>
       </c>
       <c r="B281" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C281" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
@@ -4630,10 +4818,10 @@
         <v>281</v>
       </c>
       <c r="B282" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C282" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
@@ -4642,10 +4830,10 @@
         <v>282</v>
       </c>
       <c r="B283" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C283" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
@@ -4654,10 +4842,10 @@
         <v>283</v>
       </c>
       <c r="B284" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C284" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
@@ -4666,10 +4854,10 @@
         <v>284</v>
       </c>
       <c r="B285" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C285" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
@@ -4678,10 +4866,10 @@
         <v>285</v>
       </c>
       <c r="B286" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C286" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
@@ -4690,10 +4878,10 @@
         <v>286</v>
       </c>
       <c r="B287" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C287" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
@@ -4702,10 +4890,10 @@
         <v>287</v>
       </c>
       <c r="B288" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C288" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
@@ -4714,10 +4902,10 @@
         <v>288</v>
       </c>
       <c r="B289" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C289" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
@@ -4726,10 +4914,10 @@
         <v>289</v>
       </c>
       <c r="B290" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C290" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
@@ -4738,10 +4926,10 @@
         <v>290</v>
       </c>
       <c r="B291" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C291" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
@@ -4750,10 +4938,10 @@
         <v>291</v>
       </c>
       <c r="B292" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C292" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
@@ -4762,10 +4950,10 @@
         <v>292</v>
       </c>
       <c r="B293" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C293" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
@@ -4774,10 +4962,10 @@
         <v>293</v>
       </c>
       <c r="B294" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C294" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
@@ -4786,10 +4974,10 @@
         <v>294</v>
       </c>
       <c r="B295" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C295" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
@@ -4835,7 +5023,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4847,7 +5035,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>